<commit_message>
ajustando para sobrescrever a planilha
</commit_message>
<xml_diff>
--- a/fixtures/sheet-nova.xlsx
+++ b/fixtures/sheet-nova.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -416,52 +416,23 @@
         <v>sexo</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Lillian</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Volkman</v>
-      </c>
-      <c r="C5" t="str">
-        <v>358.207.570-25</v>
-      </c>
-      <c r="D5" t="str">
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Dominic</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Bayer</v>
+      </c>
+      <c r="C2" t="str">
+        <v>070.027.887-79</v>
+      </c>
+      <c r="D2" t="str">
         <v>Masculino</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>Carleton</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Kutch</v>
-      </c>
-      <c r="C6" t="str">
-        <v>006.075.105-36</v>
-      </c>
-      <c r="D6" t="str">
-        <v>Masculino</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>Nathaniel</v>
-      </c>
-      <c r="B7" t="str">
-        <v>Jakubowski-Cremin</v>
-      </c>
-      <c r="C7" t="str">
-        <v>161.678.066-59</v>
-      </c>
-      <c r="D7" t="str">
-        <v>Feminino</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>